<commit_message>
Adicionei os modelos Lógicos e físicos
</commit_message>
<xml_diff>
--- a/aula1Tabela.xlsx
+++ b/aula1Tabela.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\60556335317\Desktop\BancoDeDados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F552FB27-595A-46AB-80F4-7CD59BC43C41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0079E001-CDEA-4CF9-B0BB-DB0C5C7DD1B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5556" xr2:uid="{9F0A1536-0517-4970-AD64-8C25F015F739}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Aluno</t>
   </si>
@@ -82,15 +82,9 @@
     <t>São Paulo</t>
   </si>
   <si>
-    <t>SP</t>
-  </si>
-  <si>
     <t>Disciplinas</t>
   </si>
   <si>
-    <t>Matemática, Português, Inglês</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -104,13 +98,31 @@
   </si>
   <si>
     <t>Inglês</t>
+  </si>
+  <si>
+    <t>Cleide</t>
+  </si>
+  <si>
+    <t>Diadema</t>
+  </si>
+  <si>
+    <t>DisciplinasAluno</t>
+  </si>
+  <si>
+    <t>IdAluno</t>
+  </si>
+  <si>
+    <t>IdEstado</t>
+  </si>
+  <si>
+    <t>IdCidade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,8 +143,51 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF99FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCC00CC"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF8395ED"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFBF71C9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,8 +206,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0099FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -175,197 +242,66 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,8 +310,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF8395ED"/>
+      <color rgb="FFBF71C9"/>
+      <color rgb="FFFFCCFF"/>
       <color rgb="FFFF99FF"/>
-      <color rgb="FFFFCCFF"/>
+      <color rgb="FF0099FF"/>
+      <color rgb="FF66CCFF"/>
+      <color rgb="FFCCCCFF"/>
+      <color rgb="FFCC00CC"/>
+      <color rgb="FFCC66FF"/>
+      <color rgb="FFCC00FF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -686,120 +630,260 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB3BBCF-D02A-41F9-BFA2-4C2722125A83}">
-  <dimension ref="F3:N9"/>
+  <dimension ref="F4:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="12.109375" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" customWidth="1"/>
+    <col min="11" max="11" width="9.21875" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" customWidth="1"/>
     <col min="14" max="14" width="11.109375" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="6:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="6:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F4" s="11" t="s">
+    <row r="4" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="13"/>
-      <c r="M4" s="11" t="s">
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="14"/>
+    </row>
+    <row r="5" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="13"/>
-    </row>
-    <row r="5" spans="6:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F5" s="14" t="s">
+      <c r="G5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="6:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="11">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="4">
+        <v>111</v>
+      </c>
+      <c r="I6" s="21">
+        <v>1</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="9">
+        <v>1</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="15" t="s">
+      <c r="O6" s="22"/>
+    </row>
+    <row r="7" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F7" s="11">
         <v>2</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="G7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="4">
+        <v>222</v>
+      </c>
+      <c r="I7" s="21">
+        <v>2</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="9">
+        <v>2</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="K8" s="5"/>
+      <c r="L8" s="9">
         <v>3</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="M8" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="K9" s="6"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+    </row>
+    <row r="10" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F12" s="13"/>
+      <c r="G12" s="2"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F13" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="J13" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="M5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="6:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F6" s="7"/>
-      <c r="G6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="9">
-        <v>111</v>
-      </c>
-      <c r="I6" s="9" t="s">
+      <c r="K13" s="14"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="N13" s="18"/>
+    </row>
+    <row r="14" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F14" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="N14" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F15" s="15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="M6" s="7"/>
-      <c r="N6" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="6:14" x14ac:dyDescent="0.3">
-      <c r="F7" s="2"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="3"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="6:14" x14ac:dyDescent="0.3">
-      <c r="F8" s="2"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="3"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="3" t="s">
+      <c r="H15" s="20">
+        <v>1</v>
+      </c>
+      <c r="J15" s="20">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="11">
+        <v>1</v>
+      </c>
+      <c r="N15" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F16" s="15">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="6:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F9" s="4"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="6"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="6"/>
+      <c r="H16" s="20">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="11">
+        <v>1</v>
+      </c>
+      <c r="N16" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L17" s="3"/>
+      <c r="M17" s="11">
+        <v>1</v>
+      </c>
+      <c r="N17" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L18" s="3"/>
+      <c r="M18" s="11">
+        <v>2</v>
+      </c>
+      <c r="N18" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="M19" s="11">
+        <v>2</v>
+      </c>
+      <c r="N19" s="9">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="M4:N4"/>
+  <mergeCells count="5">
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="M13:N13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>